<commit_message>
feature/ADMINDASH-354: change new excel template order provided by anwari
</commit_message>
<xml_diff>
--- a/client/assets/template/templateImportOrders.xlsx
+++ b/client/assets/template/templateImportOrders.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="27320" windowHeight="13660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>PickupName</t>
   </si>
@@ -84,6 +84,9 @@
     <t>PackageWeight</t>
   </si>
   <si>
+    <t>PackageVolume</t>
+  </si>
+  <si>
     <t>WebOrderID</t>
   </si>
   <si>
@@ -99,6 +102,9 @@
     <t>PaymentType</t>
   </si>
   <si>
+    <t>UseExtraHelper</t>
+  </si>
+  <si>
     <t>PackageHeight</t>
   </si>
   <si>
@@ -160,6 +166,9 @@
   </si>
   <si>
     <t>Isinya berupa kaos. Nomor Penerima 2 : 0816100600</t>
+  </si>
+  <si>
+    <t>465776512736172000000000000000000000000</t>
   </si>
 </sst>
 </file>
@@ -167,7 +176,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -252,7 +261,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,8 +281,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -316,17 +326,26 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -344,6 +363,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -615,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,11 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -648,7 +667,7 @@
     <col min="14" max="14" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.875" style="3" customWidth="1"/>
     <col min="16" max="16" width="9.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.875" style="19" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.375" style="16" customWidth="1"/>
     <col min="19" max="19" width="8.5" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" style="3" bestFit="1" customWidth="1"/>
@@ -656,18 +675,20 @@
     <col min="22" max="22" width="11.875" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.625" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.25" style="3" customWidth="1"/>
-    <col min="26" max="26" width="34.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.25" style="3" customWidth="1"/>
-    <col min="28" max="28" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.25" style="3" customWidth="1"/>
+    <col min="27" max="27" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.25" style="3" customWidth="1"/>
     <col min="29" max="29" width="10.25" style="3" customWidth="1"/>
     <col min="30" max="30" width="10.625" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10.25" style="3" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="11.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="13.375" style="3"/>
+    <col min="33" max="33" width="11.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="13.375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="6" customFormat="1">
+    <row r="1" spans="1:34" s="6" customFormat="1">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -716,112 +737,118 @@
       <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="9" t="s">
-        <v>21</v>
+      <c r="Q1" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="R1" s="14" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Y1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="AC1" s="10" t="s">
         <v>20</v>
       </c>
       <c r="AD1" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="10" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1">
+    <row r="2" spans="1:34" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2">
         <v>88210961203</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2">
         <v>11410</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J2" s="2">
         <v>88210961203</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="N2" s="3">
         <v>12940</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>4.6577651273617203E+38</v>
+        <v>36</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="R2" s="15">
         <v>42379</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
@@ -839,17 +866,17 @@
       <c r="X2" s="1">
         <v>0</v>
       </c>
-      <c r="Y2" s="2">
-        <v>10000</v>
+      <c r="Y2" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0</v>
       </c>
       <c r="AC2" s="1">
         <v>1</v>
@@ -862,6 +889,13 @@
       </c>
       <c r="AF2" s="1">
         <v>20</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -871,6 +905,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <ignoredErrors>
+    <ignoredError sqref="Q2" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
feature/ADMINDASH-354: add new templateImportOrder new version
</commit_message>
<xml_diff>
--- a/client/assets/template/templateImportOrders.xlsx
+++ b/client/assets/template/templateImportOrders.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="your data" sheetId="1" r:id="rId1"/>
+    <sheet name="legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>PickupName</t>
   </si>
@@ -135,9 +136,6 @@
     <t>Jakarta Selatan</t>
   </si>
   <si>
-    <t>Later</t>
-  </si>
-  <si>
     <t>IsCOD</t>
   </si>
   <si>
@@ -165,10 +163,34 @@
     <t>Hati-hati barang mudah pecah.</t>
   </si>
   <si>
-    <t>Isinya berupa kaos. Nomor Penerima 2 : 0816100600</t>
-  </si>
-  <si>
     <t>465776512736172000000000000000000000000</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>LATER</t>
+  </si>
+  <si>
+    <t>NOW</t>
+  </si>
+  <si>
+    <t>REGULER</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Payment Type</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>Isinya berupa kaos. Nomor Penerima 2: 0816100600</t>
   </si>
 </sst>
 </file>
@@ -635,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -645,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -750,7 +772,7 @@
         <v>24</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V1" s="9" t="s">
         <v>25</v>
@@ -800,10 +822,10 @@
         <v>88210961203</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>34</v>
@@ -818,19 +840,19 @@
         <v>36</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="2">
         <v>88210961203</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" s="3">
         <v>12940</v>
@@ -842,38 +864,37 @@
         <v>36</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R2" s="15">
         <v>42379</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
-      <c r="U2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="W2" s="3" t="b">
-        <v>1</v>
+      <c r="U2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AB2" s="2">
         <v>0</v>
@@ -893,9 +914,8 @@
       <c r="AG2" s="1">
         <v>1</v>
       </c>
-      <c r="AH2" s="1" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+      <c r="AH2" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -909,6 +929,89 @@
     <ignoredError sqref="Q2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>legend!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>S1:S1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>legend!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>U1:W1048576 AH1:AH1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>legend!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AA1:AA1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>

<commit_message>
feature/ADMINDASH-354: change template again
</commit_message>
<xml_diff>
--- a/client/assets/template/templateImportOrders.xlsx
+++ b/client/assets/template/templateImportOrders.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840"/>
   </bookViews>
   <sheets>
-    <sheet name="your data" sheetId="1" r:id="rId1"/>
+    <sheet name="Order list" sheetId="1" r:id="rId1"/>
     <sheet name="legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -198,7 +198,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -348,6 +348,15 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -355,15 +364,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -689,8 +689,8 @@
     <col min="14" max="14" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.875" style="3" customWidth="1"/>
     <col min="16" max="16" width="9.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.875" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.375" style="16" customWidth="1"/>
+    <col min="17" max="17" width="36.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.375" style="19" customWidth="1"/>
     <col min="19" max="19" width="8.5" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.75" style="3" customWidth="1"/>
@@ -759,10 +759,10 @@
       <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="17" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="13" t="s">
@@ -863,10 +863,10 @@
       <c r="P2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="15">
+      <c r="R2" s="18">
         <v>42379</v>
       </c>
       <c r="S2" s="1" t="s">

</xml_diff>

<commit_message>
feature/ADMINDASH-354: change template from anwari
</commit_message>
<xml_diff>
--- a/client/assets/template/templateImportOrders.xlsx
+++ b/client/assets/template/templateImportOrders.xlsx
@@ -145,9 +145,6 @@
     <t>Kejora Office</t>
   </si>
   <si>
-    <t>WALLET</t>
-  </si>
-  <si>
     <t>no-reply@etobee.com</t>
   </si>
   <si>
@@ -187,10 +184,13 @@
     <t>Payment Type</t>
   </si>
   <si>
-    <t>CASH</t>
-  </si>
-  <si>
     <t>Isinya berupa kaos. Nomor Penerima 2: 0816100600</t>
+  </si>
+  <si>
+    <t>Wallet</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -840,19 +840,19 @@
         <v>36</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="2">
         <v>88210961203</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N2" s="3">
         <v>12940</v>
@@ -864,37 +864,37 @@
         <v>36</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R2" s="18">
         <v>42379</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="AB2" s="2">
         <v>0</v>
@@ -915,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -976,37 +976,37 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>